<commit_message>
skeleton done, need css
</commit_message>
<xml_diff>
--- a/createDatabase/All_Curation.xlsx
+++ b/createDatabase/All_Curation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snorl\Documents\Project\Django\createDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58543AD7-085F-4C2D-8BDF-89BB46D867C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A5ECA-1CB7-4F29-8326-FB316D1DF3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{1CBAB564-CBD3-814B-99F9-F6F557618218}"/>
+    <workbookView xWindow="43080" yWindow="5910" windowWidth="29040" windowHeight="15720" xr2:uid="{1CBAB564-CBD3-814B-99F9-F6F557618218}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="11" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14520" uniqueCount="2859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14526" uniqueCount="2859">
   <si>
     <t>Enhancer No.</t>
   </si>
@@ -9230,8 +9230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715C1BEF-F5A0-4A9D-8A7B-75C6A70E4B88}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="103" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10218,9 +10218,15 @@
       <c r="G12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="H12" s="14">
+        <v>17</v>
+      </c>
+      <c r="I12" s="14">
+        <v>48997385</v>
+      </c>
+      <c r="J12" s="14">
+        <v>49056145</v>
+      </c>
       <c r="K12" s="14" t="s">
         <v>2141</v>
       </c>
@@ -10884,9 +10890,15 @@
       <c r="G20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="H20" s="14">
+        <v>7</v>
+      </c>
+      <c r="I20" s="14">
+        <v>95608432</v>
+      </c>
+      <c r="J20" s="14">
+        <v>95609655</v>
+      </c>
       <c r="K20" s="14" t="s">
         <v>2090</v>
       </c>
@@ -10962,9 +10974,15 @@
       <c r="G21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="H21" s="14">
+        <v>4</v>
+      </c>
+      <c r="I21" s="14">
+        <v>73725619</v>
+      </c>
+      <c r="J21" s="14">
+        <v>73726851</v>
+      </c>
       <c r="K21" s="14" t="s">
         <v>2088</v>
       </c>
@@ -13357,7 +13375,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:29" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -13443,7 +13461,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:29" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -13628,8 +13646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6CEA11-5A1D-4DC3-8858-8E758B3F215C}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14978,9 +14996,15 @@
       <c r="G16" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="H16" s="14" t="s">
+        <v>2400</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>2671</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>2672</v>
+      </c>
       <c r="K16" s="14" t="s">
         <v>2206</v>
       </c>
@@ -15058,9 +15082,15 @@
       <c r="G17" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="H17" s="14" t="s">
+        <v>2400</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>2671</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>2672</v>
+      </c>
       <c r="K17" s="14" t="s">
         <v>2206</v>
       </c>
@@ -21569,7 +21599,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="63" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:28" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -21655,7 +21685,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="63" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:28" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -25301,7 +25331,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:28" ht="63" x14ac:dyDescent="0.5">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -32250,7 +32280,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="146" spans="1:29" ht="63" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:29" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A146" s="5">
         <v>145</v>
       </c>
@@ -32335,7 +32365,7 @@
       </c>
       <c r="AC146" s="5"/>
     </row>
-    <row r="147" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:29" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A147" s="5">
         <v>146</v>
       </c>
@@ -33448,7 +33478,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="160" spans="1:29" ht="157.5" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:29" ht="173.25" x14ac:dyDescent="0.5">
       <c r="A160" s="5">
         <v>159</v>
       </c>
@@ -34788,7 +34818,7 @@
       </c>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" spans="1:29" ht="126" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:29" ht="141.75" x14ac:dyDescent="0.5">
       <c r="A8" s="5">
         <v>7</v>
       </c>

</xml_diff>